<commit_message>
33. Introduction to Custom Formatting in Excel
</commit_message>
<xml_diff>
--- a/Section 4/30. Find and Select Cells That Meet Specific Conditions/Select-Special.xlsx
+++ b/Section 4/30. Find and Select Cells That Meet Specific Conditions/Select-Special.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NewPC\Desktop\Courses\Video creating\The Complete Financial Analyst Course\Resources\3. Useful Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data_science\udemy_economics\Section 4\30. Find and Select Cells That Meet Specific Conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4730AE0-E6A8-4FED-B617-7A8340953258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Select special" sheetId="1" r:id="rId1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="26">
   <si>
     <t>Select special</t>
   </si>
@@ -118,7 +119,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -191,7 +192,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -216,7 +217,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Index --&gt;"/>
@@ -589,11 +590,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="B1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -699,13 +702,21 @@
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="4">
@@ -795,13 +806,21 @@
       <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="4">

</xml_diff>